<commit_message>
feat: remove unused column from clo template
</commit_message>
<xml_diff>
--- a/public/template/clo.xlsx
+++ b/public/template/clo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inu-garden\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE63212-6CAB-4822-A04C-263F60890181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624AB173-9E61-4019-83B3-B676A2A31948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2310" windowWidth="27135" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>description</t>
   </si>
   <si>
     <t>expectedPassingAssignmentPercentage</t>
-  </si>
-  <si>
-    <t>expectedScorePercentage</t>
   </si>
   <si>
     <t>expectedPassingStudentPercentage</t>
@@ -91,7 +88,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -107,14 +104,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{126C1BD8-F5A6-457B-AFF0-70541D72B5BA}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
-  <autoFilter ref="A1:I2" xr:uid="{126C1BD8-F5A6-457B-AFF0-70541D72B5BA}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{126C1BD8-F5A6-457B-AFF0-70541D72B5BA}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{126C1BD8-F5A6-457B-AFF0-70541D72B5BA}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B98BF78B-F364-4B0E-BCDB-68D7A6827CD8}" name="_code"/>
     <tableColumn id="2" xr3:uid="{F2EAB228-4ED4-4050-BE64-C50A51B982D6}" name="weight"/>
     <tableColumn id="3" xr3:uid="{1CE7BA80-5DE3-4114-9C62-32FAFA6499DA}" name="description"/>
     <tableColumn id="4" xr3:uid="{03307266-16FF-40F6-BDA7-8354B7F4C9A7}" name="expectedPassingAssignmentPercentage"/>
-    <tableColumn id="5" xr3:uid="{762A478F-89B4-42A4-8AE5-33B521958979}" name="expectedScorePercentage"/>
     <tableColumn id="6" xr3:uid="{EDB2B363-CAC5-40A6-B2D6-6FC9A78FF7B2}" name="expectedPassingStudentPercentage"/>
     <tableColumn id="7" xr3:uid="{E6B500B7-DAFE-4AA4-BF4A-2E0E695DADCD}" name="courseId"/>
     <tableColumn id="8" xr3:uid="{606C73BB-4DFC-4870-AE86-C95F4FD50034}" name="subProgramLearningOutcomeId"/>
@@ -387,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -398,19 +394,18 @@
     <col min="1" max="2" width="10.25" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="29.25" customWidth="1"/>
-    <col min="6" max="6" width="36.875" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="31.125" customWidth="1"/>
-    <col min="9" max="9" width="30.125" customWidth="1"/>
+    <col min="5" max="5" width="36.875" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="31.125" customWidth="1"/>
+    <col min="8" max="8" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -425,13 +420,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>